<commit_message>
Filtre recherche d'offre candidat
</commit_message>
<xml_diff>
--- a/TODO_Projet_Java_Updated.xlsx
+++ b/TODO_Projet_Java_Updated.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://poce-my.sharepoint.com/personal/lucas_schwindenhammer_edu_ece_fr/Documents/Ing3/Semestre2/POO Java/projet-java-recrutement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="8_{88235350-D142-4740-9ACC-56B6C973FE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAB2EA7C-8E76-465F-BB81-F086AA0F3BEB}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="8_{88235350-D142-4740-9ACC-56B6C973FE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3870DE8-9C81-4510-9266-F3BD39A72964}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TODO" sheetId="1" r:id="rId1"/>
-    <sheet name="Reste à faire" sheetId="3" r:id="rId2"/>
-    <sheet name="Notation PowerPoint" sheetId="4" r:id="rId3"/>
-    <sheet name="Notation Démo" sheetId="5" r:id="rId4"/>
-    <sheet name="Planning" sheetId="2" r:id="rId5"/>
+    <sheet name="LIEN POWERPOINT" sheetId="6" r:id="rId1"/>
+    <sheet name="TODO" sheetId="1" r:id="rId2"/>
+    <sheet name="Reste à faire" sheetId="3" r:id="rId3"/>
+    <sheet name="Notation PowerPoint" sheetId="4" r:id="rId4"/>
+    <sheet name="Notation Démo" sheetId="5" r:id="rId5"/>
+    <sheet name="Planning" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TODO!$C$1:$C$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TODO!$C$1:$C$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4294963746" uniqueCount="4294967227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="139">
   <si>
     <t>Module</t>
   </si>
@@ -153,12 +154,6 @@
     <t>OK</t>
   </si>
   <si>
-    <t>À compléter</t>
-  </si>
-  <si>
-    <t>Manquant</t>
-  </si>
-  <si>
     <t>À vérifier</t>
   </si>
   <si>
@@ -370,12 +365,6 @@
   </si>
   <si>
     <t>Ajout bouton réfusé, voir profil dans la vue des candidatures</t>
-  </si>
-  <si>
-    <t>Ajout bouton modification profil</t>
-  </si>
-  <si>
-    <t>Ajout bouton retrait candidature</t>
   </si>
   <si>
     <t>Ajout comptage du nombre de candidatures sur un poste et afficher le nombre de candidature sur le poste</t>
@@ -728,12 +717,21 @@
   <si>
     <t>Note finale sur 24 (bornée à 20)</t>
   </si>
+  <si>
+    <t>https://poce-my.sharepoint.com/:p:/g/personal/maxime_delplace_edu_ece_fr/EVqPIiXTuDhAoCGLPn36VrsBQ0YEMGndAir2ZYsn1JG8Ew?e=Oix8az</t>
+  </si>
+  <si>
+    <t>✅</t>
+  </si>
+  <si>
+    <t>https://poce-my.sharepoint.com/:p:/g/personal/julien_bitschenauxdurand_edu_ece_fr/EeZO0dO9lYpJsj8XuQnFAooBU-PJ2FbRcP7tJ7DEdi1BYw?e=sumBMr</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -834,6 +832,30 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -975,10 +997,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1040,8 +1063,12 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1055,10 +1082,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1347,24 +1370,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE89F09-070A-4D6C-AB93-5069CEF1F743}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="141.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A3" s="23" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{7DA0D216-EAA7-4B69-93B5-8892FE977CD9}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{EABE9A13-F5D3-D74C-92FA-EF6481EEF2DF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="121" workbookViewId="0">
+    <sheetView zoomScale="121" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.44140625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="94.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="94.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1378,16 +1437,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1398,13 +1457,16 @@
         <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1415,13 +1477,16 @@
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>76</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1432,13 +1497,16 @@
         <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1449,13 +1517,16 @@
         <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1466,19 +1537,19 @@
         <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1489,13 +1560,16 @@
         <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="F7" t="s">
+        <v>59</v>
       </c>
       <c r="G7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1506,13 +1580,16 @@
         <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>81</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
       </c>
       <c r="G8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1523,19 +1600,19 @@
         <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1546,19 +1623,19 @@
         <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1566,22 +1643,22 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1592,13 +1669,16 @@
         <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>85</v>
+      </c>
+      <c r="F12" t="s">
+        <v>61</v>
       </c>
       <c r="G12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1609,19 +1689,19 @@
         <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G13">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1632,19 +1712,19 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1652,22 +1732,22 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F15" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1675,22 +1755,22 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1701,13 +1781,16 @@
         <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>92</v>
+        <v>90</v>
+      </c>
+      <c r="F17" t="s">
+        <v>61</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1718,13 +1801,16 @@
         <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>93</v>
+        <v>91</v>
+      </c>
+      <c r="F18" t="s">
+        <v>59</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1732,22 +1818,22 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G19">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1758,19 +1844,19 @@
         <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G20">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1778,22 +1864,22 @@
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G21">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1801,22 +1887,22 @@
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G22">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1827,13 +1913,16 @@
         <v>36</v>
       </c>
       <c r="E23" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="F23" t="s">
+        <v>61</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1844,13 +1933,16 @@
         <v>36</v>
       </c>
       <c r="E24" t="s">
-        <v>99</v>
+        <v>97</v>
+      </c>
+      <c r="F24" t="s">
+        <v>59</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1858,22 +1950,22 @@
         <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F25" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1881,13 +1973,13 @@
         <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F26" t="s">
         <v>57</v>
@@ -1896,7 +1988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1904,22 +1996,22 @@
         <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1927,16 +2019,16 @@
         <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E28" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F28" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G28">
         <v>2</v>
@@ -1948,189 +2040,195 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49747CC2-9CCF-44D2-AB9A-DE4AB36389C5}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScale="171" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="85.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" t="s">
         <v>105</v>
       </c>
-      <c r="B1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F55132-252C-4029-8546-4EDCA27ACD8E}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="73.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:3" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="6">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:3" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="6">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" ht="76.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:3" ht="61.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="6">
+        <v>2</v>
+      </c>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" ht="106.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F55132-252C-4029-8546-4EDCA27ACD8E}">
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="73.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C1" s="4"/>
-    </row>
-    <row r="2" spans="1:3" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" s="6">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7"/>
-    </row>
-    <row r="3" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:3" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="6">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:3" ht="135.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="6">
-        <v>6</v>
-      </c>
-      <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="6">
-        <v>2</v>
-      </c>
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:3" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B7" s="6">
-        <v>4</v>
-      </c>
-      <c r="C7" s="7"/>
-    </row>
-    <row r="8" spans="1:3" ht="76.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="6">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7"/>
-    </row>
-    <row r="9" spans="1:3" ht="61.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" s="6">
-        <v>2</v>
-      </c>
-      <c r="C9" s="7"/>
-    </row>
-    <row r="10" spans="1:3" ht="106.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B10" s="6">
-        <v>1</v>
-      </c>
-      <c r="C10" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5AE67C-AD8D-4A2B-9949-692C7E798699}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -2138,134 +2236,134 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.88671875" customWidth="1"/>
+    <col min="1" max="1" width="66.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B2" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="141.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B3" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="249" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="231" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B4" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="331.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="307.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B5" s="12">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="154.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B6" s="12">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B7" s="12">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B8" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B9" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B10" s="15">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B11" s="12">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B12" s="17">
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B13" s="17">
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B14" s="17">
         <v>-2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B15" s="17">
         <v>-2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B16" s="20">
         <v>20</v>
@@ -2276,7 +2374,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4E5F719-14BD-4FE5-A358-A0B23E18168B}">
   <dimension ref="A1:B17"/>
   <sheetViews>
@@ -2284,146 +2382,146 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>56</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>58</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>60</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>62</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>64</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>